<commit_message>
Updated burndown charts to include progress from a member
</commit_message>
<xml_diff>
--- a/deliverable3/burndown_chart/Burndown_Chart.xlsx
+++ b/deliverable3/burndown_chart/Burndown_Chart.xlsx
@@ -684,46 +684,46 @@
                   <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>71</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>67</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>58</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>52</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>52</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>52</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>50</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>50</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>50</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>46</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>46</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>46</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>46</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>46</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1302,7 +1302,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23:F29"/>
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1552,7 +1552,7 @@
         <v>61.206896551724121</v>
       </c>
       <c r="G12">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -1572,7 +1572,7 @@
         <v>58.758620689655146</v>
       </c>
       <c r="G13">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -1592,7 +1592,7 @@
         <v>56.310344827586178</v>
       </c>
       <c r="G14">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
@@ -1612,7 +1612,7 @@
         <v>53.86206896551721</v>
       </c>
       <c r="G15">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -1632,7 +1632,7 @@
         <v>51.413793103448242</v>
       </c>
       <c r="G16">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
@@ -1652,7 +1652,7 @@
         <v>48.965517241379267</v>
       </c>
       <c r="G17">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
@@ -1672,7 +1672,7 @@
         <v>46.517241379310299</v>
       </c>
       <c r="G18">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
@@ -1692,7 +1692,7 @@
         <v>44.068965517241324</v>
       </c>
       <c r="G19">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
@@ -1712,7 +1712,7 @@
         <v>41.620689655172356</v>
       </c>
       <c r="G20">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
@@ -1731,7 +1731,7 @@
         <v>39.172413793103388</v>
       </c>
       <c r="G21">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
@@ -1742,7 +1742,7 @@
         <v>36.72413793103442</v>
       </c>
       <c r="G22">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
@@ -1753,7 +1753,7 @@
         <v>34.275862068965445</v>
       </c>
       <c r="G23">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
@@ -1764,7 +1764,7 @@
         <v>31.827586206896477</v>
       </c>
       <c r="G24">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
@@ -1775,7 +1775,7 @@
         <v>29.379310344827509</v>
       </c>
       <c r="G25">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>